<commit_message>
Small routing change, added extra silkscreen labels
</commit_message>
<xml_diff>
--- a/Hardware/Electronics/Data Acquisition Board/ADC Breakout/BoM.xlsx
+++ b/Hardware/Electronics/Data Acquisition Board/ADC Breakout/BoM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willie\Documents\Uni\Newcastle\4 Fourth Year\1 Final Year Project\trunk\Hardware\Electronics\Data Acquisition Board\ADC Breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9F3375-9F5F-4A3F-823B-8A6AB71B0C49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3F69FF-656D-4966-BAC5-C50A87B60835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6508AD80-5785-495C-937B-5500FE895B69}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="DIN Plug" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DIN Plug'!$B$1:$K$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DIN Plug'!$B$1:$K$143</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="134">
   <si>
     <t xml:space="preserve">    ADC1</t>
   </si>
@@ -248,9 +248,6 @@
     <t xml:space="preserve">    R15</t>
   </si>
   <si>
-    <t xml:space="preserve">    R16</t>
-  </si>
-  <si>
     <t xml:space="preserve">    R17</t>
   </si>
   <si>
@@ -332,22 +329,10 @@
     <t>https://www.digikey.com.au/product-detail/en/panasonic-electronic-components/ERA-3AEB333V/P33KDBCT-ND/1466088</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
     <t>Digikey Part #</t>
   </si>
   <si>
     <t>RHM100DCT-ND</t>
-  </si>
-  <si>
-    <t>100 kOhms ±1% 0.25W, 1/4W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200, Pulse Withstanding Thick Film</t>
-  </si>
-  <si>
-    <t>RHM100KADCT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/rohm-semiconductor/ESR03EZPF1003/RHM100KADCT-ND/1983754</t>
   </si>
   <si>
     <t>445-5662-1-ND</t>
@@ -824,11 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE20D855-7A6D-49D9-8684-28A19F146B00}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="B1:P146"/>
+  <dimension ref="B1:P145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,37 +829,37 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>81</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" t="s">
         <v>82</v>
       </c>
-      <c r="H1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" t="s">
-        <v>83</v>
-      </c>
       <c r="K1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -895,13 +879,13 @@
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -910,7 +894,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -930,13 +914,13 @@
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -945,7 +929,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -965,13 +949,13 @@
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -980,7 +964,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1000,13 +984,13 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -1035,13 +1019,13 @@
         <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1050,7 +1034,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1070,13 +1054,13 @@
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -1085,7 +1069,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1105,13 +1089,13 @@
         <v>0</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1140,13 +1124,13 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1155,7 +1139,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1175,13 +1159,13 @@
         <v>0</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1190,7 +1174,7 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1210,13 +1194,13 @@
         <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1225,7 +1209,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1245,13 +1229,13 @@
         <v>0</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -1260,7 +1244,7 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1280,13 +1264,13 @@
         <v>0</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1295,7 +1279,7 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1315,13 +1299,13 @@
         <v>0</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1330,7 +1314,7 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1350,13 +1334,13 @@
         <v>0</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1365,7 +1349,7 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1385,13 +1369,13 @@
         <v>0</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1400,7 +1384,7 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1420,13 +1404,13 @@
         <v>0</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1435,7 +1419,7 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1455,13 +1439,13 @@
         <v>0</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1490,13 +1474,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1525,13 +1509,13 @@
         <v>0</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1540,7 +1524,7 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
@@ -1560,13 +1544,13 @@
         <v>0</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1575,7 +1559,7 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1595,13 +1579,13 @@
         <v>0</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -1610,7 +1594,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1630,13 +1614,13 @@
         <v>0</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -1645,7 +1629,7 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
@@ -1665,13 +1649,13 @@
         <v>0</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -1680,7 +1664,7 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1700,13 +1684,13 @@
         <v>0</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -1715,7 +1699,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
@@ -1735,13 +1719,13 @@
         <v>0</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -1750,7 +1734,7 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1770,13 +1754,13 @@
         <v>0</v>
       </c>
       <c r="H27" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -1785,7 +1769,7 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
@@ -1805,13 +1789,13 @@
         <v>0</v>
       </c>
       <c r="H28" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1840,13 +1824,13 @@
         <v>0</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -1855,12 +1839,12 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>15</v>
@@ -1875,13 +1859,13 @@
         <v>0</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -1890,7 +1874,7 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>39</v>
       </c>
@@ -1910,13 +1894,13 @@
         <v>0</v>
       </c>
       <c r="H31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -1945,13 +1929,13 @@
         <v>0</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -1960,7 +1944,7 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>41</v>
       </c>
@@ -1980,13 +1964,13 @@
         <v>0</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -1995,7 +1979,7 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>43</v>
       </c>
@@ -2015,13 +1999,13 @@
         <v>0</v>
       </c>
       <c r="H34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -2030,7 +2014,7 @@
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>44</v>
       </c>
@@ -2050,13 +2034,13 @@
         <v>0</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -2065,7 +2049,7 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>45</v>
       </c>
@@ -2085,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="H36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -2120,13 +2104,13 @@
         <v>0</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -2135,7 +2119,7 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
-    <row r="38" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>48</v>
       </c>
@@ -2155,13 +2139,13 @@
         <v>0</v>
       </c>
       <c r="H38" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -2170,9 +2154,9 @@
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
     </row>
-    <row r="39" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>49</v>
@@ -2190,13 +2174,13 @@
         <v>0</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -2205,15 +2189,15 @@
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E40" s="2">
         <v>1.72</v>
@@ -2225,13 +2209,13 @@
         <v>1</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -2240,15 +2224,15 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="41" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E41" s="2">
         <v>1.72</v>
@@ -2260,13 +2244,13 @@
         <v>1</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -2275,7 +2259,7 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>55</v>
       </c>
@@ -2295,13 +2279,13 @@
         <v>0</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -2310,7 +2294,7 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
     </row>
-    <row r="43" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>57</v>
       </c>
@@ -2330,13 +2314,13 @@
         <v>0</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -2345,7 +2329,7 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
     </row>
-    <row r="44" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>58</v>
       </c>
@@ -2365,13 +2349,13 @@
         <v>0</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -2380,7 +2364,7 @@
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>59</v>
       </c>
@@ -2400,13 +2384,13 @@
         <v>0</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -2415,7 +2399,7 @@
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>60</v>
       </c>
@@ -2435,13 +2419,13 @@
         <v>0</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -2450,7 +2434,7 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>61</v>
       </c>
@@ -2470,13 +2454,13 @@
         <v>0</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
@@ -2485,7 +2469,7 @@
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
     </row>
-    <row r="48" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>62</v>
       </c>
@@ -2505,13 +2489,13 @@
         <v>0</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
@@ -2520,7 +2504,7 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>63</v>
       </c>
@@ -2540,13 +2524,13 @@
         <v>0</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
@@ -2555,7 +2539,7 @@
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
     </row>
-    <row r="50" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>64</v>
       </c>
@@ -2575,13 +2559,13 @@
         <v>0</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
@@ -2590,7 +2574,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>65</v>
       </c>
@@ -2610,13 +2594,13 @@
         <v>0</v>
       </c>
       <c r="H51" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J51" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
@@ -2625,7 +2609,7 @@
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
     </row>
-    <row r="52" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>67</v>
       </c>
@@ -2645,13 +2629,13 @@
         <v>0</v>
       </c>
       <c r="H52" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -2660,7 +2644,7 @@
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
     </row>
-    <row r="53" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>68</v>
       </c>
@@ -2680,13 +2664,13 @@
         <v>0</v>
       </c>
       <c r="H53" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J53" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
@@ -2695,7 +2679,7 @@
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
     </row>
-    <row r="54" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>69</v>
       </c>
@@ -2715,13 +2699,13 @@
         <v>0</v>
       </c>
       <c r="H54" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
@@ -2730,18 +2714,18 @@
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
     </row>
-    <row r="55" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E55" s="2">
-        <v>0.21</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F55" s="2">
         <v>1</v>
@@ -2749,14 +2733,14 @@
       <c r="G55" s="2">
         <v>0</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>102</v>
+      <c r="H55" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
@@ -2765,18 +2749,18 @@
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
     </row>
-    <row r="56" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="E56" s="2">
-        <v>0.55000000000000004</v>
+        <v>1.04</v>
       </c>
       <c r="F56" s="2">
         <v>1</v>
@@ -2784,14 +2768,14 @@
       <c r="G56" s="2">
         <v>0</v>
       </c>
-      <c r="H56" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>111</v>
+      <c r="H56" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -2800,18 +2784,18 @@
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
     </row>
-    <row r="57" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="E57" s="2">
-        <v>1.04</v>
+        <v>1.56</v>
       </c>
       <c r="F57" s="2">
         <v>1</v>
@@ -2820,13 +2804,13 @@
         <v>0</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
@@ -2835,34 +2819,16 @@
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
     </row>
-    <row r="58" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E58" s="2">
-        <v>1.56</v>
-      </c>
-      <c r="F58" s="2">
-        <v>1</v>
-      </c>
-      <c r="G58" s="2">
-        <v>0</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>115</v>
-      </c>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="4"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
@@ -2870,7 +2836,7 @@
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
     </row>
-    <row r="59" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2887,7 +2853,7 @@
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
     </row>
-    <row r="60" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2904,7 +2870,7 @@
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
     </row>
-    <row r="61" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2921,7 +2887,7 @@
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
     </row>
-    <row r="62" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2938,7 +2904,7 @@
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
     </row>
-    <row r="63" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -2955,7 +2921,7 @@
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
     </row>
-    <row r="64" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2972,15 +2938,15 @@
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
     </row>
-    <row r="65" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
       <c r="J65" s="4"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
@@ -2989,7 +2955,7 @@
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
     </row>
-    <row r="66" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -3006,7 +2972,7 @@
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
     </row>
-    <row r="67" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -3023,7 +2989,7 @@
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
     </row>
-    <row r="68" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -3040,7 +3006,7 @@
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
     </row>
-    <row r="69" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -3057,7 +3023,7 @@
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
     </row>
-    <row r="70" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -3074,7 +3040,7 @@
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
     </row>
-    <row r="71" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -3091,7 +3057,7 @@
       <c r="O71" s="2"/>
       <c r="P71" s="2"/>
     </row>
-    <row r="72" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -3108,15 +3074,15 @@
       <c r="O72" s="2"/>
       <c r="P72" s="2"/>
     </row>
-    <row r="73" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
       <c r="J73" s="4"/>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
@@ -3125,15 +3091,15 @@
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
     </row>
-    <row r="74" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
       <c r="J74" s="4"/>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
@@ -3142,7 +3108,7 @@
       <c r="O74" s="2"/>
       <c r="P74" s="2"/>
     </row>
-    <row r="75" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -3159,7 +3125,7 @@
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
     </row>
-    <row r="76" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -3176,7 +3142,7 @@
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>
     </row>
-    <row r="77" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
@@ -3193,7 +3159,7 @@
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
     </row>
-    <row r="78" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -3210,7 +3176,7 @@
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
     </row>
-    <row r="79" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
@@ -3227,7 +3193,7 @@
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
     </row>
-    <row r="80" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
@@ -3244,7 +3210,7 @@
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
     </row>
-    <row r="81" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -3261,7 +3227,7 @@
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
     </row>
-    <row r="82" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -3278,7 +3244,7 @@
       <c r="O82" s="2"/>
       <c r="P82" s="2"/>
     </row>
-    <row r="83" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -3295,7 +3261,7 @@
       <c r="O83" s="2"/>
       <c r="P83" s="2"/>
     </row>
-    <row r="84" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -3312,7 +3278,7 @@
       <c r="O84" s="2"/>
       <c r="P84" s="2"/>
     </row>
-    <row r="85" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -3329,7 +3295,7 @@
       <c r="O85" s="2"/>
       <c r="P85" s="2"/>
     </row>
-    <row r="86" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
@@ -3346,15 +3312,15 @@
       <c r="O86" s="2"/>
       <c r="P86" s="2"/>
     </row>
-    <row r="87" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
       <c r="J87" s="4"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
@@ -3363,15 +3329,15 @@
       <c r="O87" s="2"/>
       <c r="P87" s="2"/>
     </row>
-    <row r="88" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
       <c r="J88" s="4"/>
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
@@ -3380,7 +3346,7 @@
       <c r="O88" s="2"/>
       <c r="P88" s="2"/>
     </row>
-    <row r="89" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -3397,7 +3363,7 @@
       <c r="O89" s="2"/>
       <c r="P89" s="2"/>
     </row>
-    <row r="90" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
@@ -3414,7 +3380,7 @@
       <c r="O90" s="2"/>
       <c r="P90" s="2"/>
     </row>
-    <row r="91" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
@@ -3431,7 +3397,7 @@
       <c r="O91" s="2"/>
       <c r="P91" s="2"/>
     </row>
-    <row r="92" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -3448,7 +3414,7 @@
       <c r="O92" s="2"/>
       <c r="P92" s="2"/>
     </row>
-    <row r="93" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -3465,7 +3431,7 @@
       <c r="O93" s="2"/>
       <c r="P93" s="2"/>
     </row>
-    <row r="94" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -3482,7 +3448,7 @@
       <c r="O94" s="2"/>
       <c r="P94" s="2"/>
     </row>
-    <row r="95" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -3499,15 +3465,15 @@
       <c r="O95" s="2"/>
       <c r="P95" s="2"/>
     </row>
-    <row r="96" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
       <c r="J96" s="4"/>
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
@@ -3516,7 +3482,7 @@
       <c r="O96" s="2"/>
       <c r="P96" s="2"/>
     </row>
-    <row r="97" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -3533,15 +3499,15 @@
       <c r="O97" s="2"/>
       <c r="P97" s="2"/>
     </row>
-    <row r="98" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
       <c r="J98" s="4"/>
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
@@ -3550,7 +3516,7 @@
       <c r="O98" s="2"/>
       <c r="P98" s="2"/>
     </row>
-    <row r="99" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -3567,7 +3533,7 @@
       <c r="O99" s="2"/>
       <c r="P99" s="2"/>
     </row>
-    <row r="100" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -3584,15 +3550,15 @@
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
     </row>
-    <row r="101" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
       <c r="J101" s="4"/>
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
@@ -3601,15 +3567,15 @@
       <c r="O101" s="2"/>
       <c r="P101" s="2"/>
     </row>
-    <row r="102" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
       <c r="J102" s="4"/>
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
@@ -3618,7 +3584,7 @@
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
     </row>
-    <row r="103" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
@@ -3635,7 +3601,7 @@
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
     </row>
-    <row r="104" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -3652,7 +3618,7 @@
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
     </row>
-    <row r="105" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -3669,7 +3635,7 @@
       <c r="O105" s="2"/>
       <c r="P105" s="2"/>
     </row>
-    <row r="106" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -3686,7 +3652,7 @@
       <c r="O106" s="2"/>
       <c r="P106" s="2"/>
     </row>
-    <row r="107" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
@@ -3703,7 +3669,7 @@
       <c r="O107" s="2"/>
       <c r="P107" s="2"/>
     </row>
-    <row r="108" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -3720,7 +3686,7 @@
       <c r="O108" s="2"/>
       <c r="P108" s="2"/>
     </row>
-    <row r="109" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -3737,7 +3703,7 @@
       <c r="O109" s="2"/>
       <c r="P109" s="2"/>
     </row>
-    <row r="110" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
@@ -3754,7 +3720,7 @@
       <c r="O110" s="2"/>
       <c r="P110" s="2"/>
     </row>
-    <row r="111" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -3763,7 +3729,7 @@
       <c r="G111" s="2"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
-      <c r="J111" s="4"/>
+      <c r="J111" s="2"/>
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
@@ -3771,16 +3737,16 @@
       <c r="O111" s="2"/>
       <c r="P111" s="2"/>
     </row>
-    <row r="112" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
-      <c r="H112" s="3"/>
-      <c r="I112" s="3"/>
-      <c r="J112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="4"/>
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
       <c r="M112" s="2"/>
@@ -3788,7 +3754,7 @@
       <c r="O112" s="2"/>
       <c r="P112" s="2"/>
     </row>
-    <row r="113" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -3805,7 +3771,7 @@
       <c r="O113" s="2"/>
       <c r="P113" s="2"/>
     </row>
-    <row r="114" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -3822,15 +3788,15 @@
       <c r="O114" s="2"/>
       <c r="P114" s="2"/>
     </row>
-    <row r="115" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
       <c r="J115" s="4"/>
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
@@ -3839,7 +3805,7 @@
       <c r="O115" s="2"/>
       <c r="P115" s="2"/>
     </row>
-    <row r="116" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -3856,7 +3822,7 @@
       <c r="O116" s="2"/>
       <c r="P116" s="2"/>
     </row>
-    <row r="117" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
@@ -3865,7 +3831,7 @@
       <c r="G117" s="2"/>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
-      <c r="J117" s="4"/>
+      <c r="J117" s="2"/>
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
       <c r="M117" s="2"/>
@@ -3873,7 +3839,7 @@
       <c r="O117" s="2"/>
       <c r="P117" s="2"/>
     </row>
-    <row r="118" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -3890,7 +3856,7 @@
       <c r="O118" s="2"/>
       <c r="P118" s="2"/>
     </row>
-    <row r="119" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
@@ -3907,7 +3873,7 @@
       <c r="O119" s="2"/>
       <c r="P119" s="2"/>
     </row>
-    <row r="120" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -3924,7 +3890,7 @@
       <c r="O120" s="2"/>
       <c r="P120" s="2"/>
     </row>
-    <row r="121" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -3941,7 +3907,7 @@
       <c r="O121" s="2"/>
       <c r="P121" s="2"/>
     </row>
-    <row r="122" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -3958,7 +3924,7 @@
       <c r="O122" s="2"/>
       <c r="P122" s="2"/>
     </row>
-    <row r="123" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -3975,7 +3941,7 @@
       <c r="O123" s="2"/>
       <c r="P123" s="2"/>
     </row>
-    <row r="124" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
@@ -3992,7 +3958,7 @@
       <c r="O124" s="2"/>
       <c r="P124" s="2"/>
     </row>
-    <row r="125" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
@@ -4009,7 +3975,7 @@
       <c r="O125" s="2"/>
       <c r="P125" s="2"/>
     </row>
-    <row r="126" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -4018,7 +3984,7 @@
       <c r="G126" s="2"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
-      <c r="J126" s="2"/>
+      <c r="J126" s="4"/>
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
       <c r="M126" s="2"/>
@@ -4026,7 +3992,7 @@
       <c r="O126" s="2"/>
       <c r="P126" s="2"/>
     </row>
-    <row r="127" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -4043,7 +4009,7 @@
       <c r="O127" s="2"/>
       <c r="P127" s="2"/>
     </row>
-    <row r="128" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
@@ -4060,7 +4026,7 @@
       <c r="O128" s="2"/>
       <c r="P128" s="2"/>
     </row>
-    <row r="129" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
@@ -4077,7 +4043,7 @@
       <c r="O129" s="2"/>
       <c r="P129" s="2"/>
     </row>
-    <row r="130" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
@@ -4094,7 +4060,7 @@
       <c r="O130" s="2"/>
       <c r="P130" s="2"/>
     </row>
-    <row r="131" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
@@ -4111,7 +4077,7 @@
       <c r="O131" s="2"/>
       <c r="P131" s="2"/>
     </row>
-    <row r="132" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
@@ -4128,7 +4094,7 @@
       <c r="O132" s="2"/>
       <c r="P132" s="2"/>
     </row>
-    <row r="133" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
@@ -4145,7 +4111,7 @@
       <c r="O133" s="2"/>
       <c r="P133" s="2"/>
     </row>
-    <row r="134" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
@@ -4162,7 +4128,7 @@
       <c r="O134" s="2"/>
       <c r="P134" s="2"/>
     </row>
-    <row r="135" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
@@ -4179,7 +4145,7 @@
       <c r="O135" s="2"/>
       <c r="P135" s="2"/>
     </row>
-    <row r="136" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
@@ -4196,7 +4162,7 @@
       <c r="O136" s="2"/>
       <c r="P136" s="2"/>
     </row>
-    <row r="137" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
@@ -4213,7 +4179,7 @@
       <c r="O137" s="2"/>
       <c r="P137" s="2"/>
     </row>
-    <row r="138" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
@@ -4230,7 +4196,7 @@
       <c r="O138" s="2"/>
       <c r="P138" s="2"/>
     </row>
-    <row r="139" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
@@ -4247,7 +4213,7 @@
       <c r="O139" s="2"/>
       <c r="P139" s="2"/>
     </row>
-    <row r="140" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
@@ -4264,7 +4230,7 @@
       <c r="O140" s="2"/>
       <c r="P140" s="2"/>
     </row>
-    <row r="141" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
@@ -4281,15 +4247,15 @@
       <c r="O141" s="2"/>
       <c r="P141" s="2"/>
     </row>
-    <row r="142" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
-      <c r="H142" s="3"/>
-      <c r="I142" s="3"/>
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
       <c r="J142" s="4"/>
       <c r="K142" s="2"/>
       <c r="L142" s="2"/>
@@ -4298,7 +4264,7 @@
       <c r="O142" s="2"/>
       <c r="P142" s="2"/>
     </row>
-    <row r="143" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
@@ -4307,7 +4273,7 @@
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
-      <c r="J143" s="4"/>
+      <c r="J143" s="2"/>
       <c r="K143" s="2"/>
       <c r="L143" s="2"/>
       <c r="M143" s="2"/>
@@ -4315,7 +4281,7 @@
       <c r="O143" s="2"/>
       <c r="P143" s="2"/>
     </row>
-    <row r="144" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
@@ -4349,32 +4315,10 @@
       <c r="O145" s="2"/>
       <c r="P145" s="2"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
-      <c r="D146" s="2"/>
-      <c r="E146" s="2"/>
-      <c r="F146" s="2"/>
-      <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
-      <c r="I146" s="2"/>
-      <c r="J146" s="2"/>
-      <c r="K146" s="2"/>
-      <c r="L146" s="2"/>
-      <c r="M146" s="2"/>
-      <c r="N146" s="2"/>
-      <c r="O146" s="2"/>
-      <c r="P146" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:K144" xr:uid="{5E607A6A-E149-4D76-B4A2-B81B2BAF4324}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="0.1uF"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K144">
-      <sortCondition ref="I1:I144"/>
+  <autoFilter ref="B1:K143" xr:uid="{5E607A6A-E149-4D76-B4A2-B81B2BAF4324}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K143">
+      <sortCondition ref="I1:I143"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -4382,60 +4326,59 @@
     <hyperlink ref="J29" r:id="rId2" xr:uid="{69DF0938-DC81-409F-8696-BE067E8DD990}"/>
     <hyperlink ref="J32" r:id="rId3" xr:uid="{3302D50F-340F-40F6-956B-B76D19D50066}"/>
     <hyperlink ref="J37" r:id="rId4" xr:uid="{8CBF4D71-5DC1-4664-8C97-F290F7AF19BC}"/>
-    <hyperlink ref="J55" r:id="rId5" xr:uid="{700F7384-E9C8-4CB3-BF2D-1D6DAC313192}"/>
-    <hyperlink ref="J20" r:id="rId6" xr:uid="{34C59EB2-F43B-4799-A5ED-FC974A27277C}"/>
-    <hyperlink ref="J19" r:id="rId7" xr:uid="{D9009194-AFB3-4CAA-8003-A4A378A4B804}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{4AF8C100-4776-412B-B6E0-276144CB6F91}"/>
-    <hyperlink ref="J6" r:id="rId9" xr:uid="{876D5AF4-1C46-42FA-A283-5861B5613CDC}"/>
-    <hyperlink ref="J3" r:id="rId10" xr:uid="{128B00A9-254C-4D64-820A-8856059A2FA6}"/>
-    <hyperlink ref="J5" r:id="rId11" xr:uid="{B0C1FFFB-89C3-49D0-AF86-68B2F9CE1B24}"/>
-    <hyperlink ref="J33" r:id="rId12" xr:uid="{C7E466A7-6DFF-44B8-9E4B-A268701DA002}"/>
-    <hyperlink ref="J8" r:id="rId13" xr:uid="{A8C17366-3A76-4F2D-BE96-B282FDEB03A4}"/>
-    <hyperlink ref="J10" r:id="rId14" xr:uid="{93E295C2-BF85-4F3F-B3D3-0DDEF2CC8B36}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{585CE7EE-E7E6-42AC-BD8A-7904CD3A5175}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{6154A14B-007E-4AB4-BE3A-15D536171D62}"/>
-    <hyperlink ref="J30" r:id="rId17" xr:uid="{D8B09EBB-5EB9-43D5-B265-B069BA3AA2E4}"/>
-    <hyperlink ref="J23" r:id="rId18" xr:uid="{478F2756-3950-4F2C-BC89-3E824D0E9C01}"/>
-    <hyperlink ref="J21" r:id="rId19" xr:uid="{103A239E-29B9-421A-91D7-41572D06DAF9}"/>
-    <hyperlink ref="J7" r:id="rId20" xr:uid="{0A60759E-2ABD-42D5-84AF-66AEDAE2AAE8}"/>
-    <hyperlink ref="J4" r:id="rId21" xr:uid="{C1F56A8F-77E0-483B-A168-E96D82C31473}"/>
-    <hyperlink ref="J13" r:id="rId22" xr:uid="{ECC7D7DB-B458-488B-95AC-65DE2C46EEBC}"/>
-    <hyperlink ref="J14" r:id="rId23" xr:uid="{D8B20778-2001-4566-9493-3924D9647B0C}"/>
-    <hyperlink ref="J27" r:id="rId24" xr:uid="{E88249B4-4CB8-4D11-AEFD-2FCFBCE7231F}"/>
-    <hyperlink ref="J28" r:id="rId25" xr:uid="{D8677954-49C7-4E2D-9657-1D29D649D223}"/>
-    <hyperlink ref="J31" r:id="rId26" xr:uid="{851A022E-DB67-4F51-B01D-42A52F8526DE}"/>
-    <hyperlink ref="J34" r:id="rId27" xr:uid="{C4B7302C-C490-4E81-8289-62FD7DF7C4B5}"/>
-    <hyperlink ref="J35" r:id="rId28" xr:uid="{06351768-4BFC-4EB3-A077-78A6A68F4EC2}"/>
-    <hyperlink ref="J36" r:id="rId29" xr:uid="{DE8EE7CB-958E-4E06-98FD-07E10A1AC638}"/>
-    <hyperlink ref="J38" r:id="rId30" xr:uid="{437B6AD5-8175-4367-9A75-4C2EA00D966D}"/>
-    <hyperlink ref="J42" r:id="rId31" xr:uid="{3205D0F1-B037-4C3F-8C8C-61EF0EB7C6D3}"/>
-    <hyperlink ref="J43" r:id="rId32" xr:uid="{38874B4B-335A-4069-9C4A-D652698705F2}"/>
-    <hyperlink ref="J44" r:id="rId33" xr:uid="{B0F0D94F-1FAE-4433-B38E-11CFBF9977AC}"/>
-    <hyperlink ref="J45" r:id="rId34" xr:uid="{372B53E1-ECC8-40E9-ABF3-BB89965894B0}"/>
-    <hyperlink ref="J46" r:id="rId35" xr:uid="{62110228-C0D7-4F03-B8D0-3E92AF09886E}"/>
-    <hyperlink ref="J47" r:id="rId36" xr:uid="{90DA16DA-AE04-40CA-9E6A-5E2D318FE646}"/>
-    <hyperlink ref="J48" r:id="rId37" xr:uid="{790149FE-74A2-4234-A0D6-0269FE3188AA}"/>
-    <hyperlink ref="J49" r:id="rId38" xr:uid="{9E3A7BB8-09D4-49BB-A53C-37B05B0B4C65}"/>
-    <hyperlink ref="J50" r:id="rId39" xr:uid="{F1775819-CBDD-4AD3-8332-A88E555FC12F}"/>
-    <hyperlink ref="J11" r:id="rId40" xr:uid="{816C38AB-3A08-4B14-9DAF-D31215C1F6FC}"/>
-    <hyperlink ref="J12" r:id="rId41" xr:uid="{99FED5CB-922C-4B8E-92E3-E7DDFCAD0BDD}"/>
-    <hyperlink ref="J15" r:id="rId42" xr:uid="{EB83497A-7F22-4592-8C65-86F71457A00D}"/>
-    <hyperlink ref="J18" r:id="rId43" xr:uid="{852F13C9-167A-4BB5-BD2C-01DB05C23BA2}"/>
-    <hyperlink ref="J22" r:id="rId44" xr:uid="{4F96DF9C-CDEE-4425-8236-18CFFF8A1136}"/>
-    <hyperlink ref="J24" r:id="rId45" xr:uid="{F060ACF8-B54C-4049-A902-03A2E936011E}"/>
-    <hyperlink ref="J25" r:id="rId46" xr:uid="{00E026CD-C9ED-4F10-8DC1-9909EF6384D6}"/>
-    <hyperlink ref="J26" r:id="rId47" xr:uid="{423B0A5E-5257-48F6-BEA2-E2EFFD91BBDE}"/>
-    <hyperlink ref="J52" r:id="rId48" xr:uid="{F7A8C23B-54DC-45F7-AAFD-C8BE63141B95}"/>
-    <hyperlink ref="J53" r:id="rId49" xr:uid="{97E2D958-FBF9-4CCA-89D5-AFDFA74997D7}"/>
-    <hyperlink ref="J54" r:id="rId50" xr:uid="{E0C5BF63-AF11-4F1C-AA28-05685601BB4D}"/>
-    <hyperlink ref="J56" r:id="rId51" xr:uid="{DB26FDA2-23A2-4582-9F98-2A32303FFE32}"/>
-    <hyperlink ref="J40" r:id="rId52" xr:uid="{506636AB-2DCD-4CA0-B718-56467E08FF5C}"/>
-    <hyperlink ref="J41" r:id="rId53" xr:uid="{A5D4CBA5-BF75-4924-A55D-979AE1AB441C}"/>
-    <hyperlink ref="J58" r:id="rId54" xr:uid="{8EBDBC95-AB00-4DD7-BC90-5A0A32F12C40}"/>
-    <hyperlink ref="J39" r:id="rId55" xr:uid="{E2226C1A-DFEC-4413-9371-7999B849A7E2}"/>
-    <hyperlink ref="J57" r:id="rId56" xr:uid="{271997BE-5926-40DB-89D0-46BA4F6A1BF2}"/>
+    <hyperlink ref="J20" r:id="rId5" xr:uid="{34C59EB2-F43B-4799-A5ED-FC974A27277C}"/>
+    <hyperlink ref="J19" r:id="rId6" xr:uid="{D9009194-AFB3-4CAA-8003-A4A378A4B804}"/>
+    <hyperlink ref="J9" r:id="rId7" xr:uid="{4AF8C100-4776-412B-B6E0-276144CB6F91}"/>
+    <hyperlink ref="J6" r:id="rId8" xr:uid="{876D5AF4-1C46-42FA-A283-5861B5613CDC}"/>
+    <hyperlink ref="J3" r:id="rId9" xr:uid="{128B00A9-254C-4D64-820A-8856059A2FA6}"/>
+    <hyperlink ref="J5" r:id="rId10" xr:uid="{B0C1FFFB-89C3-49D0-AF86-68B2F9CE1B24}"/>
+    <hyperlink ref="J33" r:id="rId11" xr:uid="{C7E466A7-6DFF-44B8-9E4B-A268701DA002}"/>
+    <hyperlink ref="J8" r:id="rId12" xr:uid="{A8C17366-3A76-4F2D-BE96-B282FDEB03A4}"/>
+    <hyperlink ref="J10" r:id="rId13" xr:uid="{93E295C2-BF85-4F3F-B3D3-0DDEF2CC8B36}"/>
+    <hyperlink ref="J16" r:id="rId14" xr:uid="{585CE7EE-E7E6-42AC-BD8A-7904CD3A5175}"/>
+    <hyperlink ref="J17" r:id="rId15" xr:uid="{6154A14B-007E-4AB4-BE3A-15D536171D62}"/>
+    <hyperlink ref="J30" r:id="rId16" xr:uid="{D8B09EBB-5EB9-43D5-B265-B069BA3AA2E4}"/>
+    <hyperlink ref="J23" r:id="rId17" xr:uid="{478F2756-3950-4F2C-BC89-3E824D0E9C01}"/>
+    <hyperlink ref="J21" r:id="rId18" xr:uid="{103A239E-29B9-421A-91D7-41572D06DAF9}"/>
+    <hyperlink ref="J7" r:id="rId19" xr:uid="{0A60759E-2ABD-42D5-84AF-66AEDAE2AAE8}"/>
+    <hyperlink ref="J4" r:id="rId20" xr:uid="{C1F56A8F-77E0-483B-A168-E96D82C31473}"/>
+    <hyperlink ref="J13" r:id="rId21" xr:uid="{ECC7D7DB-B458-488B-95AC-65DE2C46EEBC}"/>
+    <hyperlink ref="J14" r:id="rId22" xr:uid="{D8B20778-2001-4566-9493-3924D9647B0C}"/>
+    <hyperlink ref="J27" r:id="rId23" xr:uid="{E88249B4-4CB8-4D11-AEFD-2FCFBCE7231F}"/>
+    <hyperlink ref="J28" r:id="rId24" xr:uid="{D8677954-49C7-4E2D-9657-1D29D649D223}"/>
+    <hyperlink ref="J31" r:id="rId25" xr:uid="{851A022E-DB67-4F51-B01D-42A52F8526DE}"/>
+    <hyperlink ref="J34" r:id="rId26" xr:uid="{C4B7302C-C490-4E81-8289-62FD7DF7C4B5}"/>
+    <hyperlink ref="J35" r:id="rId27" xr:uid="{06351768-4BFC-4EB3-A077-78A6A68F4EC2}"/>
+    <hyperlink ref="J36" r:id="rId28" xr:uid="{DE8EE7CB-958E-4E06-98FD-07E10A1AC638}"/>
+    <hyperlink ref="J38" r:id="rId29" xr:uid="{437B6AD5-8175-4367-9A75-4C2EA00D966D}"/>
+    <hyperlink ref="J42" r:id="rId30" xr:uid="{3205D0F1-B037-4C3F-8C8C-61EF0EB7C6D3}"/>
+    <hyperlink ref="J43" r:id="rId31" xr:uid="{38874B4B-335A-4069-9C4A-D652698705F2}"/>
+    <hyperlink ref="J44" r:id="rId32" xr:uid="{B0F0D94F-1FAE-4433-B38E-11CFBF9977AC}"/>
+    <hyperlink ref="J45" r:id="rId33" xr:uid="{372B53E1-ECC8-40E9-ABF3-BB89965894B0}"/>
+    <hyperlink ref="J46" r:id="rId34" xr:uid="{62110228-C0D7-4F03-B8D0-3E92AF09886E}"/>
+    <hyperlink ref="J47" r:id="rId35" xr:uid="{90DA16DA-AE04-40CA-9E6A-5E2D318FE646}"/>
+    <hyperlink ref="J48" r:id="rId36" xr:uid="{790149FE-74A2-4234-A0D6-0269FE3188AA}"/>
+    <hyperlink ref="J49" r:id="rId37" xr:uid="{9E3A7BB8-09D4-49BB-A53C-37B05B0B4C65}"/>
+    <hyperlink ref="J50" r:id="rId38" xr:uid="{F1775819-CBDD-4AD3-8332-A88E555FC12F}"/>
+    <hyperlink ref="J11" r:id="rId39" xr:uid="{816C38AB-3A08-4B14-9DAF-D31215C1F6FC}"/>
+    <hyperlink ref="J12" r:id="rId40" xr:uid="{99FED5CB-922C-4B8E-92E3-E7DDFCAD0BDD}"/>
+    <hyperlink ref="J15" r:id="rId41" xr:uid="{EB83497A-7F22-4592-8C65-86F71457A00D}"/>
+    <hyperlink ref="J18" r:id="rId42" xr:uid="{852F13C9-167A-4BB5-BD2C-01DB05C23BA2}"/>
+    <hyperlink ref="J22" r:id="rId43" xr:uid="{4F96DF9C-CDEE-4425-8236-18CFFF8A1136}"/>
+    <hyperlink ref="J24" r:id="rId44" xr:uid="{F060ACF8-B54C-4049-A902-03A2E936011E}"/>
+    <hyperlink ref="J25" r:id="rId45" xr:uid="{00E026CD-C9ED-4F10-8DC1-9909EF6384D6}"/>
+    <hyperlink ref="J26" r:id="rId46" xr:uid="{423B0A5E-5257-48F6-BEA2-E2EFFD91BBDE}"/>
+    <hyperlink ref="J52" r:id="rId47" xr:uid="{F7A8C23B-54DC-45F7-AAFD-C8BE63141B95}"/>
+    <hyperlink ref="J53" r:id="rId48" xr:uid="{97E2D958-FBF9-4CCA-89D5-AFDFA74997D7}"/>
+    <hyperlink ref="J54" r:id="rId49" xr:uid="{E0C5BF63-AF11-4F1C-AA28-05685601BB4D}"/>
+    <hyperlink ref="J55" r:id="rId50" xr:uid="{DB26FDA2-23A2-4582-9F98-2A32303FFE32}"/>
+    <hyperlink ref="J40" r:id="rId51" xr:uid="{506636AB-2DCD-4CA0-B718-56467E08FF5C}"/>
+    <hyperlink ref="J41" r:id="rId52" xr:uid="{A5D4CBA5-BF75-4924-A55D-979AE1AB441C}"/>
+    <hyperlink ref="J57" r:id="rId53" xr:uid="{8EBDBC95-AB00-4DD7-BC90-5A0A32F12C40}"/>
+    <hyperlink ref="J39" r:id="rId54" xr:uid="{E2226C1A-DFEC-4413-9371-7999B849A7E2}"/>
+    <hyperlink ref="J56" r:id="rId55" xr:uid="{271997BE-5926-40DB-89D0-46BA4F6A1BF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId57"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId56"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ADC BREAKOUT ASSEMBLY TAG
</commit_message>
<xml_diff>
--- a/Hardware/Electronics/Data Acquisition Board/ADC Breakout/BoM.xlsx
+++ b/Hardware/Electronics/Data Acquisition Board/ADC Breakout/BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willie\Documents\Uni\Newcastle\4 Fourth Year\1 Final Year Project\trunk\Hardware\Electronics\Data Acquisition Board\ADC Breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3F69FF-656D-4966-BAC5-C50A87B60835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB754D8-F40D-4A23-969C-EEF9BAEA1150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6508AD80-5785-495C-937B-5500FE895B69}"/>
+    <workbookView xWindow="0" yWindow="7770" windowWidth="28800" windowHeight="7830" xr2:uid="{6508AD80-5785-495C-937B-5500FE895B69}"/>
   </bookViews>
   <sheets>
     <sheet name="DIN Plug" sheetId="2" r:id="rId1"/>
@@ -338,12 +338,6 @@
     <t>445-5662-1-ND</t>
   </si>
   <si>
-    <t>10µF ±20% 6.3V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>1276-1119-1-ND</t>
-  </si>
-  <si>
     <t>311-1080-1-ND</t>
   </si>
   <si>
@@ -416,9 +410,6 @@
     <t>https://www.digikey.com.au/product-detail/en/tdk-corporation/CGA3E2X7R1H103K080AA/445-5662-1-ND/2443702</t>
   </si>
   <si>
-    <t>https://www.digikey.com.au/product-detail/en/samsung-electro-mechanics/CL10A106MQ8NNNC/1276-1119-1-ND/3889205</t>
-  </si>
-  <si>
     <t>https://www.digikey.com.au/product-detail/en/yageo/CC0603KRX7R9BB102/311-1080-1-ND/302990</t>
   </si>
   <si>
@@ -438,6 +429,15 @@
   </si>
   <si>
     <t>Linear Voltage Regulator IC  1 Output  300mA SOT-223-5</t>
+  </si>
+  <si>
+    <t>10µF ±10% 10V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>490-10474-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/murata-electronics/GRM188R61A106KE69D/490-10474-1-ND/5026392</t>
   </si>
 </sst>
 </file>
@@ -812,7 +812,7 @@
   <dimension ref="B1:P145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+      <selection activeCell="E30" sqref="E30:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +856,7 @@
         <v>82</v>
       </c>
       <c r="K1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
@@ -882,10 +882,10 @@
         <v>84</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -914,13 +914,13 @@
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -940,7 +940,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="2">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -949,13 +949,13 @@
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -984,13 +984,13 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -1019,13 +1019,13 @@
         <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1045,7 +1045,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="2">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -1054,13 +1054,13 @@
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -1095,7 +1095,7 @@
         <v>99</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1124,13 +1124,13 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1165,7 +1165,7 @@
         <v>99</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1197,7 +1197,7 @@
         <v>86</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>85</v>
@@ -1232,7 +1232,7 @@
         <v>86</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>85</v>
@@ -1267,10 +1267,10 @@
         <v>90</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1302,10 +1302,10 @@
         <v>90</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1337,7 +1337,7 @@
         <v>86</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>85</v>
@@ -1375,7 +1375,7 @@
         <v>99</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1410,7 +1410,7 @@
         <v>99</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1442,7 +1442,7 @@
         <v>86</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>85</v>
@@ -1474,13 +1474,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1509,13 +1509,13 @@
         <v>0</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1535,7 +1535,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="2">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -1544,13 +1544,13 @@
         <v>0</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1582,7 +1582,7 @@
         <v>86</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>85</v>
@@ -1605,7 +1605,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="2">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>
@@ -1614,13 +1614,13 @@
         <v>0</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -1652,7 +1652,7 @@
         <v>86</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>85</v>
@@ -1687,7 +1687,7 @@
         <v>86</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>85</v>
@@ -1722,7 +1722,7 @@
         <v>86</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>85</v>
@@ -1757,7 +1757,7 @@
         <v>87</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>88</v>
@@ -1792,7 +1792,7 @@
         <v>87</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>88</v>
@@ -1824,13 +1824,13 @@
         <v>0</v>
       </c>
       <c r="H29" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -1844,13 +1844,13 @@
         <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="2">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F30" s="2">
         <v>1</v>
@@ -1859,13 +1859,13 @@
         <v>0</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -1897,7 +1897,7 @@
         <v>87</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>88</v>
@@ -1929,13 +1929,13 @@
         <v>0</v>
       </c>
       <c r="H32" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -1964,13 +1964,13 @@
         <v>0</v>
       </c>
       <c r="H33" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -2002,7 +2002,7 @@
         <v>87</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>88</v>
@@ -2037,7 +2037,7 @@
         <v>87</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>88</v>
@@ -2072,7 +2072,7 @@
         <v>87</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>88</v>
@@ -2104,13 +2104,13 @@
         <v>0</v>
       </c>
       <c r="H37" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -2142,7 +2142,7 @@
         <v>87</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>88</v>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>49</v>
@@ -2177,10 +2177,10 @@
         <v>91</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -2194,10 +2194,10 @@
         <v>51</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E40" s="2">
         <v>1.72</v>
@@ -2209,13 +2209,13 @@
         <v>1</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -2229,10 +2229,10 @@
         <v>52</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E41" s="2">
         <v>1.72</v>
@@ -2244,13 +2244,13 @@
         <v>1</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -2282,10 +2282,10 @@
         <v>94</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -2317,10 +2317,10 @@
         <v>94</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -2352,10 +2352,10 @@
         <v>94</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -2387,10 +2387,10 @@
         <v>94</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -2422,10 +2422,10 @@
         <v>94</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -2457,10 +2457,10 @@
         <v>94</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
@@ -2492,10 +2492,10 @@
         <v>94</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
@@ -2527,10 +2527,10 @@
         <v>94</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
@@ -2562,10 +2562,10 @@
         <v>94</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
@@ -2632,7 +2632,7 @@
         <v>95</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>96</v>
@@ -2667,7 +2667,7 @@
         <v>95</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>96</v>
@@ -2702,7 +2702,7 @@
         <v>95</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>96</v>
@@ -2737,7 +2737,7 @@
         <v>95</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>96</v>
@@ -2769,13 +2769,13 @@
         <v>0</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -2804,13 +2804,13 @@
         <v>0</v>
       </c>
       <c r="H57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J57" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
@@ -4337,46 +4337,46 @@
     <hyperlink ref="J10" r:id="rId13" xr:uid="{93E295C2-BF85-4F3F-B3D3-0DDEF2CC8B36}"/>
     <hyperlink ref="J16" r:id="rId14" xr:uid="{585CE7EE-E7E6-42AC-BD8A-7904CD3A5175}"/>
     <hyperlink ref="J17" r:id="rId15" xr:uid="{6154A14B-007E-4AB4-BE3A-15D536171D62}"/>
-    <hyperlink ref="J30" r:id="rId16" xr:uid="{D8B09EBB-5EB9-43D5-B265-B069BA3AA2E4}"/>
-    <hyperlink ref="J23" r:id="rId17" xr:uid="{478F2756-3950-4F2C-BC89-3E824D0E9C01}"/>
-    <hyperlink ref="J21" r:id="rId18" xr:uid="{103A239E-29B9-421A-91D7-41572D06DAF9}"/>
-    <hyperlink ref="J7" r:id="rId19" xr:uid="{0A60759E-2ABD-42D5-84AF-66AEDAE2AAE8}"/>
-    <hyperlink ref="J4" r:id="rId20" xr:uid="{C1F56A8F-77E0-483B-A168-E96D82C31473}"/>
-    <hyperlink ref="J13" r:id="rId21" xr:uid="{ECC7D7DB-B458-488B-95AC-65DE2C46EEBC}"/>
-    <hyperlink ref="J14" r:id="rId22" xr:uid="{D8B20778-2001-4566-9493-3924D9647B0C}"/>
-    <hyperlink ref="J27" r:id="rId23" xr:uid="{E88249B4-4CB8-4D11-AEFD-2FCFBCE7231F}"/>
-    <hyperlink ref="J28" r:id="rId24" xr:uid="{D8677954-49C7-4E2D-9657-1D29D649D223}"/>
-    <hyperlink ref="J31" r:id="rId25" xr:uid="{851A022E-DB67-4F51-B01D-42A52F8526DE}"/>
-    <hyperlink ref="J34" r:id="rId26" xr:uid="{C4B7302C-C490-4E81-8289-62FD7DF7C4B5}"/>
-    <hyperlink ref="J35" r:id="rId27" xr:uid="{06351768-4BFC-4EB3-A077-78A6A68F4EC2}"/>
-    <hyperlink ref="J36" r:id="rId28" xr:uid="{DE8EE7CB-958E-4E06-98FD-07E10A1AC638}"/>
-    <hyperlink ref="J38" r:id="rId29" xr:uid="{437B6AD5-8175-4367-9A75-4C2EA00D966D}"/>
-    <hyperlink ref="J42" r:id="rId30" xr:uid="{3205D0F1-B037-4C3F-8C8C-61EF0EB7C6D3}"/>
-    <hyperlink ref="J43" r:id="rId31" xr:uid="{38874B4B-335A-4069-9C4A-D652698705F2}"/>
-    <hyperlink ref="J44" r:id="rId32" xr:uid="{B0F0D94F-1FAE-4433-B38E-11CFBF9977AC}"/>
-    <hyperlink ref="J45" r:id="rId33" xr:uid="{372B53E1-ECC8-40E9-ABF3-BB89965894B0}"/>
-    <hyperlink ref="J46" r:id="rId34" xr:uid="{62110228-C0D7-4F03-B8D0-3E92AF09886E}"/>
-    <hyperlink ref="J47" r:id="rId35" xr:uid="{90DA16DA-AE04-40CA-9E6A-5E2D318FE646}"/>
-    <hyperlink ref="J48" r:id="rId36" xr:uid="{790149FE-74A2-4234-A0D6-0269FE3188AA}"/>
-    <hyperlink ref="J49" r:id="rId37" xr:uid="{9E3A7BB8-09D4-49BB-A53C-37B05B0B4C65}"/>
-    <hyperlink ref="J50" r:id="rId38" xr:uid="{F1775819-CBDD-4AD3-8332-A88E555FC12F}"/>
-    <hyperlink ref="J11" r:id="rId39" xr:uid="{816C38AB-3A08-4B14-9DAF-D31215C1F6FC}"/>
-    <hyperlink ref="J12" r:id="rId40" xr:uid="{99FED5CB-922C-4B8E-92E3-E7DDFCAD0BDD}"/>
-    <hyperlink ref="J15" r:id="rId41" xr:uid="{EB83497A-7F22-4592-8C65-86F71457A00D}"/>
-    <hyperlink ref="J18" r:id="rId42" xr:uid="{852F13C9-167A-4BB5-BD2C-01DB05C23BA2}"/>
-    <hyperlink ref="J22" r:id="rId43" xr:uid="{4F96DF9C-CDEE-4425-8236-18CFFF8A1136}"/>
-    <hyperlink ref="J24" r:id="rId44" xr:uid="{F060ACF8-B54C-4049-A902-03A2E936011E}"/>
-    <hyperlink ref="J25" r:id="rId45" xr:uid="{00E026CD-C9ED-4F10-8DC1-9909EF6384D6}"/>
-    <hyperlink ref="J26" r:id="rId46" xr:uid="{423B0A5E-5257-48F6-BEA2-E2EFFD91BBDE}"/>
-    <hyperlink ref="J52" r:id="rId47" xr:uid="{F7A8C23B-54DC-45F7-AAFD-C8BE63141B95}"/>
-    <hyperlink ref="J53" r:id="rId48" xr:uid="{97E2D958-FBF9-4CCA-89D5-AFDFA74997D7}"/>
-    <hyperlink ref="J54" r:id="rId49" xr:uid="{E0C5BF63-AF11-4F1C-AA28-05685601BB4D}"/>
-    <hyperlink ref="J55" r:id="rId50" xr:uid="{DB26FDA2-23A2-4582-9F98-2A32303FFE32}"/>
-    <hyperlink ref="J40" r:id="rId51" xr:uid="{506636AB-2DCD-4CA0-B718-56467E08FF5C}"/>
-    <hyperlink ref="J41" r:id="rId52" xr:uid="{A5D4CBA5-BF75-4924-A55D-979AE1AB441C}"/>
-    <hyperlink ref="J57" r:id="rId53" xr:uid="{8EBDBC95-AB00-4DD7-BC90-5A0A32F12C40}"/>
-    <hyperlink ref="J39" r:id="rId54" xr:uid="{E2226C1A-DFEC-4413-9371-7999B849A7E2}"/>
-    <hyperlink ref="J56" r:id="rId55" xr:uid="{271997BE-5926-40DB-89D0-46BA4F6A1BF2}"/>
+    <hyperlink ref="J13" r:id="rId16" xr:uid="{ECC7D7DB-B458-488B-95AC-65DE2C46EEBC}"/>
+    <hyperlink ref="J14" r:id="rId17" xr:uid="{D8B20778-2001-4566-9493-3924D9647B0C}"/>
+    <hyperlink ref="J27" r:id="rId18" xr:uid="{E88249B4-4CB8-4D11-AEFD-2FCFBCE7231F}"/>
+    <hyperlink ref="J28" r:id="rId19" xr:uid="{D8677954-49C7-4E2D-9657-1D29D649D223}"/>
+    <hyperlink ref="J31" r:id="rId20" xr:uid="{851A022E-DB67-4F51-B01D-42A52F8526DE}"/>
+    <hyperlink ref="J34" r:id="rId21" xr:uid="{C4B7302C-C490-4E81-8289-62FD7DF7C4B5}"/>
+    <hyperlink ref="J35" r:id="rId22" xr:uid="{06351768-4BFC-4EB3-A077-78A6A68F4EC2}"/>
+    <hyperlink ref="J36" r:id="rId23" xr:uid="{DE8EE7CB-958E-4E06-98FD-07E10A1AC638}"/>
+    <hyperlink ref="J38" r:id="rId24" xr:uid="{437B6AD5-8175-4367-9A75-4C2EA00D966D}"/>
+    <hyperlink ref="J42" r:id="rId25" xr:uid="{3205D0F1-B037-4C3F-8C8C-61EF0EB7C6D3}"/>
+    <hyperlink ref="J43" r:id="rId26" xr:uid="{38874B4B-335A-4069-9C4A-D652698705F2}"/>
+    <hyperlink ref="J44" r:id="rId27" xr:uid="{B0F0D94F-1FAE-4433-B38E-11CFBF9977AC}"/>
+    <hyperlink ref="J45" r:id="rId28" xr:uid="{372B53E1-ECC8-40E9-ABF3-BB89965894B0}"/>
+    <hyperlink ref="J46" r:id="rId29" xr:uid="{62110228-C0D7-4F03-B8D0-3E92AF09886E}"/>
+    <hyperlink ref="J47" r:id="rId30" xr:uid="{90DA16DA-AE04-40CA-9E6A-5E2D318FE646}"/>
+    <hyperlink ref="J48" r:id="rId31" xr:uid="{790149FE-74A2-4234-A0D6-0269FE3188AA}"/>
+    <hyperlink ref="J49" r:id="rId32" xr:uid="{9E3A7BB8-09D4-49BB-A53C-37B05B0B4C65}"/>
+    <hyperlink ref="J50" r:id="rId33" xr:uid="{F1775819-CBDD-4AD3-8332-A88E555FC12F}"/>
+    <hyperlink ref="J11" r:id="rId34" xr:uid="{816C38AB-3A08-4B14-9DAF-D31215C1F6FC}"/>
+    <hyperlink ref="J12" r:id="rId35" xr:uid="{99FED5CB-922C-4B8E-92E3-E7DDFCAD0BDD}"/>
+    <hyperlink ref="J15" r:id="rId36" xr:uid="{EB83497A-7F22-4592-8C65-86F71457A00D}"/>
+    <hyperlink ref="J18" r:id="rId37" xr:uid="{852F13C9-167A-4BB5-BD2C-01DB05C23BA2}"/>
+    <hyperlink ref="J22" r:id="rId38" xr:uid="{4F96DF9C-CDEE-4425-8236-18CFFF8A1136}"/>
+    <hyperlink ref="J24" r:id="rId39" xr:uid="{F060ACF8-B54C-4049-A902-03A2E936011E}"/>
+    <hyperlink ref="J25" r:id="rId40" xr:uid="{00E026CD-C9ED-4F10-8DC1-9909EF6384D6}"/>
+    <hyperlink ref="J26" r:id="rId41" xr:uid="{423B0A5E-5257-48F6-BEA2-E2EFFD91BBDE}"/>
+    <hyperlink ref="J52" r:id="rId42" xr:uid="{F7A8C23B-54DC-45F7-AAFD-C8BE63141B95}"/>
+    <hyperlink ref="J53" r:id="rId43" xr:uid="{97E2D958-FBF9-4CCA-89D5-AFDFA74997D7}"/>
+    <hyperlink ref="J54" r:id="rId44" xr:uid="{E0C5BF63-AF11-4F1C-AA28-05685601BB4D}"/>
+    <hyperlink ref="J55" r:id="rId45" xr:uid="{DB26FDA2-23A2-4582-9F98-2A32303FFE32}"/>
+    <hyperlink ref="J40" r:id="rId46" xr:uid="{506636AB-2DCD-4CA0-B718-56467E08FF5C}"/>
+    <hyperlink ref="J41" r:id="rId47" xr:uid="{A5D4CBA5-BF75-4924-A55D-979AE1AB441C}"/>
+    <hyperlink ref="J57" r:id="rId48" xr:uid="{8EBDBC95-AB00-4DD7-BC90-5A0A32F12C40}"/>
+    <hyperlink ref="J39" r:id="rId49" xr:uid="{E2226C1A-DFEC-4413-9371-7999B849A7E2}"/>
+    <hyperlink ref="J56" r:id="rId50" xr:uid="{271997BE-5926-40DB-89D0-46BA4F6A1BF2}"/>
+    <hyperlink ref="J4" r:id="rId51" xr:uid="{FA7C1E52-9DF4-4C23-8FC8-3BB8E7D4EBF2}"/>
+    <hyperlink ref="J7" r:id="rId52" xr:uid="{F06F5BAB-67F7-4305-BC27-041AE9694687}"/>
+    <hyperlink ref="J21" r:id="rId53" xr:uid="{0C9E8E56-F333-4F66-9D59-00451943CC87}"/>
+    <hyperlink ref="J23" r:id="rId54" xr:uid="{FF059F55-25BB-4786-9A03-FCCF21418D73}"/>
+    <hyperlink ref="J30" r:id="rId55" xr:uid="{8374DB7F-7A2D-4239-8939-FEC3B404C69C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId56"/>

</xml_diff>

<commit_message>
Reran plotting the schematic
</commit_message>
<xml_diff>
--- a/Hardware/Electronics/Data Acquisition Board/ADC Breakout/BoM.xlsx
+++ b/Hardware/Electronics/Data Acquisition Board/ADC Breakout/BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willie\Documents\Uni\Newcastle\4 Fourth Year\1 Final Year Project\trunk\Hardware\Electronics\Data Acquisition Board\ADC Breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB754D8-F40D-4A23-969C-EEF9BAEA1150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7E9C28-539B-4EA8-86F3-33D0F7F3AACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7770" windowWidth="28800" windowHeight="7830" xr2:uid="{6508AD80-5785-495C-937B-5500FE895B69}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6508AD80-5785-495C-937B-5500FE895B69}"/>
   </bookViews>
   <sheets>
     <sheet name="DIN Plug" sheetId="2" r:id="rId1"/>
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE20D855-7A6D-49D9-8684-28A19F146B00}">
   <dimension ref="B1:P145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:J30"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2823,7 +2823,10 @@
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+      <c r="E58" s="2">
+        <f>SUM(E2:E57)</f>
+        <v>36.619999999999997</v>
+      </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>

</xml_diff>